<commit_message>
the last commit for second way which is better
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ArianaGrande</t>
+          <t>JackNickelson</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Drake</t>
+          <t>ShaquilleO'Neal</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rihanna</t>
+          <t>Drake</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,10 +496,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JackNickelson</t>
+          <t>Rihanna</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ArianaGrande</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Absent</t>
         </is>

</xml_diff>